<commit_message>
Add two compressed data
</commit_message>
<xml_diff>
--- a/ethylene/data/ethylene_data.xlsx
+++ b/ethylene/data/ethylene_data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="19890" windowHeight="8985" tabRatio="719"/>
+    <workbookView windowWidth="19890" windowHeight="9405" tabRatio="719" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="CCmd" sheetId="1" r:id="rId1"/>
@@ -105,6 +105,12 @@
     <t>z07</t>
   </si>
   <si>
+    <t>z08</t>
+  </si>
+  <si>
+    <t>z09</t>
+  </si>
+  <si>
     <t>a</t>
   </si>
   <si>
@@ -121,12 +127,6 @@
   </si>
   <si>
     <t>vol</t>
-  </si>
-  <si>
-    <t>z08</t>
-  </si>
-  <si>
-    <t>z09</t>
   </si>
 </sst>
 </file>
@@ -134,10 +134,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="21">
     <font>
@@ -145,6 +145,20 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -163,6 +177,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF006100"/>
       <name val="Calibri"/>
@@ -170,10 +192,65 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -185,54 +262,30 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
-      <sz val="15"/>
+      <sz val="18"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -245,59 +298,6 @@
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -308,174 +308,180 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -483,12 +489,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -511,13 +511,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
       <top style="thin">
-        <color theme="4"/>
+        <color rgb="FF3F3F3F"/>
       </top>
-      <bottom style="double">
-        <color theme="4"/>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -537,17 +541,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -569,6 +567,17 @@
     <border>
       <left/>
       <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top/>
       <bottom style="double">
         <color rgb="FFFF8001"/>
@@ -576,174 +585,165 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FF7F7F7F"/>
       </left>
       <right style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FF7F7F7F"/>
       </right>
       <top style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FF7F7F7F"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="16" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="15" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="21" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="21" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="29" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="8" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1090,10 +1090,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:F10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.75" outlineLevelCol="5"/>
@@ -1271,11 +1271,29 @@
         <v>-32.311747</v>
       </c>
     </row>
-    <row r="9" spans="2:5">
+    <row r="9" spans="1:5">
+      <c r="A9" s="1" t="s">
+        <v>12</v>
+      </c>
       <c r="B9"/>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
+      <c r="C9" s="1">
+        <v>0.68</v>
+      </c>
+      <c r="D9" s="1">
+        <v>-32.204805</v>
+      </c>
       <c r="E9"/>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C10" s="1">
+        <v>0.55</v>
+      </c>
+      <c r="D10" s="1">
+        <v>-31.850052</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
@@ -1300,7 +1318,7 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B1">
         <v>29.3096749</v>
@@ -1312,7 +1330,7 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B2">
         <v>29.8913799</v>
@@ -1324,7 +1342,7 @@
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B3">
         <v>30.495898</v>
@@ -1417,8 +1435,8 @@
   <sheetPr/>
   <dimension ref="A1:F15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5:C11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.75" outlineLevelCol="5"/>
@@ -1434,18 +1452,18 @@
         <v>2</v>
       </c>
       <c r="C1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="D1" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="E1" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B2" s="2">
         <v>-18.143411</v>
@@ -1468,7 +1486,7 @@
     </row>
     <row r="3" spans="1:6">
       <c r="A3" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B3" s="2">
         <v>-18.228197</v>
@@ -1491,7 +1509,7 @@
     </row>
     <row r="4" spans="1:6">
       <c r="A4" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B4" s="2">
         <v>-18.306019</v>
@@ -1675,14 +1693,14 @@
     </row>
     <row r="12" spans="1:6">
       <c r="A12" s="1" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="B12" s="3">
-        <v>-17.280557</v>
+        <v>-64.40961</v>
       </c>
       <c r="C12">
         <f t="shared" si="0"/>
-        <v>-8.6402785</v>
+        <v>-32.204805</v>
       </c>
       <c r="D12" s="1">
         <v>0.68</v>
@@ -1698,14 +1716,14 @@
     </row>
     <row r="13" spans="1:6">
       <c r="A13" s="1" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="B13" s="3">
-        <v>-13.935363</v>
+        <v>-63.700104</v>
       </c>
       <c r="C13">
         <f t="shared" si="0"/>
-        <v>-6.9676815</v>
+        <v>-31.850052</v>
       </c>
       <c r="D13" s="1">
         <v>0.55</v>

</xml_diff>

<commit_message>
Update QM plot for ethylene
</commit_message>
<xml_diff>
--- a/ethylene/data/ethylene_data.xlsx
+++ b/ethylene/data/ethylene_data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="19890" windowHeight="9405" tabRatio="719" activeTab="2"/>
+    <workbookView windowWidth="19890" windowHeight="9405" tabRatio="719"/>
   </bookViews>
   <sheets>
     <sheet name="CCmd" sheetId="1" r:id="rId1"/>
@@ -12,7 +12,7 @@
     <sheet name="draft-QM" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="ExternalData_1" localSheetId="0">CCmd!$D$2:$D$8</definedName>
+    <definedName name="ExternalData_1" localSheetId="0">CCmd!$D$3:$D$9</definedName>
     <definedName name="ExternalData_1" localSheetId="1">'draft-phonon'!$B$1:$B$9</definedName>
   </definedNames>
   <calcPr calcId="144525" concurrentCalc="0"/>
@@ -151,19 +151,19 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -178,17 +178,17 @@
     </font>
     <font>
       <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -200,6 +200,82 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color theme="3"/>
@@ -208,47 +284,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -256,44 +293,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -314,13 +314,85 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -332,13 +404,67 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -350,139 +476,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -502,26 +502,26 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top/>
       <bottom style="medium">
         <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -544,8 +544,19 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -567,183 +578,172 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
       <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FF3F3F3F"/>
       </left>
       <right style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FF3F3F3F"/>
       </right>
       <top style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FF3F3F3F"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="22" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="29" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="29" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="16" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="29" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="8" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1090,10 +1090,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="A1:F10"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.75" outlineLevelCol="5"/>
@@ -1124,176 +1124,188 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
-      <c r="A2" s="1" t="s">
-        <v>5</v>
-      </c>
+    <row r="2" spans="2:6">
       <c r="B2">
-        <v>130.2452</v>
+        <v>132.850104</v>
       </c>
       <c r="C2" s="1">
-        <v>1</v>
-      </c>
-      <c r="D2">
-        <v>-32.308937</v>
+        <v>1.02</v>
+      </c>
+      <c r="D2" s="1">
+        <v>-32.305627</v>
       </c>
       <c r="E2">
         <v>0</v>
       </c>
       <c r="F2" s="1">
-        <f t="shared" ref="F2:F7" si="0">D2+E2</f>
-        <v>-32.308937</v>
+        <f>D2+E2</f>
+        <v>-32.305627</v>
       </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B3">
-        <v>131.2452</v>
+        <v>130.2452</v>
       </c>
       <c r="C3" s="1">
-        <v>0.98</v>
+        <v>1</v>
       </c>
       <c r="D3">
-        <v>-32.311858</v>
+        <v>-32.308937</v>
       </c>
       <c r="E3">
         <v>0</v>
       </c>
       <c r="F3" s="1">
-        <f t="shared" si="0"/>
-        <v>-32.311858</v>
+        <f t="shared" ref="F3:F8" si="0">D3+E3</f>
+        <v>-32.308937</v>
       </c>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B4">
-        <v>132.2452</v>
+        <v>127.640296</v>
       </c>
       <c r="C4" s="1">
-        <v>0.96</v>
+        <v>0.98</v>
       </c>
       <c r="D4">
-        <v>-32.314062</v>
+        <v>-32.311858</v>
       </c>
       <c r="E4">
         <v>0</v>
       </c>
       <c r="F4" s="1">
         <f t="shared" si="0"/>
-        <v>-32.314062</v>
+        <v>-32.311858</v>
       </c>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B5">
-        <v>133.2452</v>
+        <v>125.035392</v>
       </c>
       <c r="C5" s="1">
-        <v>0.94</v>
+        <v>0.96</v>
       </c>
       <c r="D5">
-        <v>-32.3160085</v>
+        <v>-32.314062</v>
       </c>
       <c r="E5">
         <v>0</v>
       </c>
       <c r="F5" s="1">
         <f t="shared" si="0"/>
-        <v>-32.3160085</v>
+        <v>-32.314062</v>
       </c>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B6">
-        <v>134.2452</v>
+        <v>122.430488</v>
       </c>
       <c r="C6" s="1">
-        <v>0.92</v>
+        <v>0.94</v>
       </c>
       <c r="D6">
-        <v>-32.317202</v>
+        <v>-32.3160085</v>
       </c>
       <c r="E6">
         <v>0</v>
       </c>
       <c r="F6" s="1">
         <f t="shared" si="0"/>
-        <v>-32.317202</v>
+        <v>-32.3160085</v>
       </c>
     </row>
     <row r="7" spans="1:6">
       <c r="A7" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B7">
-        <v>135.2452</v>
+        <v>119.825584</v>
       </c>
       <c r="C7" s="1">
-        <v>0.9</v>
+        <v>0.92</v>
       </c>
       <c r="D7">
-        <v>-32.3173525</v>
+        <v>-32.317202</v>
       </c>
       <c r="E7">
         <v>0</v>
       </c>
       <c r="F7" s="1">
         <f t="shared" si="0"/>
-        <v>-32.3173525</v>
+        <v>-32.317202</v>
       </c>
     </row>
     <row r="8" spans="1:6">
       <c r="A8" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B8">
-        <v>136.2452</v>
+        <v>117.22068</v>
       </c>
       <c r="C8" s="1">
-        <v>0.84</v>
+        <v>0.9</v>
       </c>
       <c r="D8">
-        <v>-32.311747</v>
+        <v>-32.3173525</v>
       </c>
       <c r="E8">
         <v>0</v>
       </c>
       <c r="F8" s="1">
-        <f>E8+D8</f>
+        <f t="shared" si="0"/>
+        <v>-32.3173525</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9">
+        <v>109.405968</v>
+      </c>
+      <c r="C9" s="1">
+        <v>0.84</v>
+      </c>
+      <c r="D9">
         <v>-32.311747</v>
       </c>
-    </row>
-    <row r="9" spans="1:5">
-      <c r="A9" s="1" t="s">
+      <c r="E9">
+        <v>0</v>
+      </c>
+      <c r="F9" s="1">
+        <f>E9+D9</f>
+        <v>-32.311747</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B9"/>
-      <c r="C9" s="1">
-        <v>0.68</v>
-      </c>
-      <c r="D9" s="1">
-        <v>-32.204805</v>
-      </c>
-      <c r="E9"/>
-    </row>
-    <row r="10" spans="1:4">
-      <c r="A10" s="1" t="s">
+      <c r="B10"/>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
+      <c r="E10"/>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C10" s="1">
-        <v>0.55</v>
-      </c>
-      <c r="D10" s="1">
-        <v>-31.850052</v>
-      </c>
+      <c r="B11"/>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
+      <c r="E11"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
@@ -1433,18 +1445,18 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="A1:F15"/>
+  <dimension ref="A1:G15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E4" sqref="E4:E11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.75" outlineLevelCol="5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.75" outlineLevelCol="6"/>
   <cols>
     <col min="2" max="2" width="9.5"/>
     <col min="3" max="3" width="11.5"/>
-    <col min="5" max="5" width="10.375"/>
-    <col min="6" max="6" width="12.625"/>
+    <col min="5" max="5" width="11.5"/>
+    <col min="6" max="7" width="12.625"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:5">
@@ -1476,8 +1488,8 @@
         <v>1.06</v>
       </c>
       <c r="E2">
-        <f>$D2*6.33163</f>
-        <v>6.7115278</v>
+        <f>$D2*130.2452</f>
+        <v>138.059912</v>
       </c>
       <c r="F2">
         <f>D2^(1/3)</f>
@@ -1499,38 +1511,42 @@
         <v>1.04</v>
       </c>
       <c r="E3">
-        <f t="shared" ref="E3:E13" si="1">$D3*6.33163</f>
-        <v>6.5848952</v>
+        <f>$D3*130.2452</f>
+        <v>135.455008</v>
       </c>
       <c r="F3">
-        <f t="shared" ref="F3:F15" si="2">D3^(1/3)</f>
+        <f t="shared" ref="F3:F15" si="1">D3^(1/3)</f>
         <v>1.01315940382018</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:7">
       <c r="A4" s="1" t="s">
         <v>16</v>
       </c>
       <c r="B4" s="2">
-        <v>-18.306019</v>
+        <v>-64.611254</v>
       </c>
       <c r="C4">
         <f t="shared" si="0"/>
-        <v>-9.1530095</v>
+        <v>-32.305627</v>
       </c>
       <c r="D4" s="1">
         <v>1.02</v>
       </c>
       <c r="E4">
+        <f>$D4*130.2452</f>
+        <v>132.850104</v>
+      </c>
+      <c r="F4">
         <f t="shared" si="1"/>
-        <v>6.4582626</v>
-      </c>
-      <c r="F4">
-        <f t="shared" si="2"/>
         <v>1.00662270956011</v>
       </c>
-    </row>
-    <row r="5" spans="1:6">
+      <c r="G4">
+        <f>B4/2</f>
+        <v>-32.305627</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
       <c r="A5" s="1" t="s">
         <v>5</v>
       </c>
@@ -1545,15 +1561,19 @@
         <v>1</v>
       </c>
       <c r="E5">
+        <f t="shared" ref="E5:E13" si="2">$D5*130.2452</f>
+        <v>130.2452</v>
+      </c>
+      <c r="F5">
         <f t="shared" si="1"/>
-        <v>6.33163</v>
-      </c>
-      <c r="F5">
-        <f t="shared" si="2"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:6">
+      <c r="G5">
+        <f t="shared" ref="G5:G13" si="3">B5/2</f>
+        <v>-32.308937</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
       <c r="A6" s="1" t="s">
         <v>6</v>
       </c>
@@ -1568,15 +1588,19 @@
         <v>0.98</v>
       </c>
       <c r="E6">
+        <f t="shared" si="2"/>
+        <v>127.640296</v>
+      </c>
+      <c r="F6">
         <f t="shared" si="1"/>
-        <v>6.2049974</v>
-      </c>
-      <c r="F6">
-        <f t="shared" si="2"/>
         <v>0.993288388379269</v>
       </c>
-    </row>
-    <row r="7" spans="1:6">
+      <c r="G6">
+        <f t="shared" si="3"/>
+        <v>-32.311858</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
       <c r="A7" s="1" t="s">
         <v>7</v>
       </c>
@@ -1591,15 +1615,19 @@
         <v>0.96</v>
       </c>
       <c r="E7">
+        <f t="shared" si="2"/>
+        <v>125.035392</v>
+      </c>
+      <c r="F7">
         <f t="shared" si="1"/>
-        <v>6.0783648</v>
-      </c>
-      <c r="F7">
-        <f t="shared" si="2"/>
         <v>0.986484829732188</v>
       </c>
-    </row>
-    <row r="8" spans="1:6">
+      <c r="G7">
+        <f t="shared" si="3"/>
+        <v>-32.314062</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
       <c r="A8" s="1" t="s">
         <v>8</v>
       </c>
@@ -1614,15 +1642,19 @@
         <v>0.94</v>
       </c>
       <c r="E8">
+        <f t="shared" si="2"/>
+        <v>122.430488</v>
+      </c>
+      <c r="F8">
         <f t="shared" si="1"/>
-        <v>5.9517322</v>
-      </c>
-      <c r="F8">
-        <f t="shared" si="2"/>
         <v>0.979586108715562</v>
       </c>
-    </row>
-    <row r="9" spans="1:6">
+      <c r="G8">
+        <f t="shared" si="3"/>
+        <v>-32.3160085</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
       <c r="A9" s="1" t="s">
         <v>9</v>
       </c>
@@ -1637,15 +1669,19 @@
         <v>0.92</v>
       </c>
       <c r="E9">
+        <f t="shared" si="2"/>
+        <v>119.825584</v>
+      </c>
+      <c r="F9">
         <f t="shared" si="1"/>
-        <v>5.8250996</v>
-      </c>
-      <c r="F9">
-        <f t="shared" si="2"/>
         <v>0.972588826218856</v>
       </c>
-    </row>
-    <row r="10" spans="1:6">
+      <c r="G9">
+        <f t="shared" si="3"/>
+        <v>-32.317202</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
       <c r="A10" s="1" t="s">
         <v>10</v>
       </c>
@@ -1660,15 +1696,19 @@
         <v>0.9</v>
       </c>
       <c r="E10">
+        <f t="shared" si="2"/>
+        <v>117.22068</v>
+      </c>
+      <c r="F10">
         <f t="shared" si="1"/>
-        <v>5.698467</v>
-      </c>
-      <c r="F10">
-        <f t="shared" si="2"/>
         <v>0.96548938460563</v>
       </c>
-    </row>
-    <row r="11" spans="1:6">
+      <c r="G10">
+        <f t="shared" si="3"/>
+        <v>-32.3173525</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
       <c r="A11" s="1" t="s">
         <v>11</v>
       </c>
@@ -1683,15 +1723,19 @@
         <v>0.84</v>
       </c>
       <c r="E11">
+        <f t="shared" si="2"/>
+        <v>109.405968</v>
+      </c>
+      <c r="F11">
         <f t="shared" si="1"/>
-        <v>5.3185692</v>
-      </c>
-      <c r="F11">
-        <f t="shared" si="2"/>
         <v>0.943538796063307</v>
       </c>
-    </row>
-    <row r="12" spans="1:6">
+      <c r="G11">
+        <f t="shared" si="3"/>
+        <v>-32.311747</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
       <c r="A12" s="1" t="s">
         <v>12</v>
       </c>
@@ -1706,15 +1750,19 @@
         <v>0.68</v>
       </c>
       <c r="E12">
+        <f t="shared" si="2"/>
+        <v>88.566736</v>
+      </c>
+      <c r="F12">
         <f t="shared" si="1"/>
-        <v>4.3055084</v>
-      </c>
-      <c r="F12">
-        <f t="shared" si="2"/>
         <v>0.879365934431636</v>
       </c>
-    </row>
-    <row r="13" spans="1:6">
+      <c r="G12">
+        <f t="shared" si="3"/>
+        <v>-32.204805</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
       <c r="A13" s="1" t="s">
         <v>13</v>
       </c>
@@ -1729,12 +1777,16 @@
         <v>0.55</v>
       </c>
       <c r="E13">
+        <f t="shared" si="2"/>
+        <v>71.63486</v>
+      </c>
+      <c r="F13">
         <f t="shared" si="1"/>
-        <v>3.4823965</v>
-      </c>
-      <c r="F13">
-        <f t="shared" si="2"/>
         <v>0.819321270600646</v>
+      </c>
+      <c r="G13">
+        <f t="shared" si="3"/>
+        <v>-31.850052</v>
       </c>
     </row>
     <row r="14" spans="4:4">

</xml_diff>